<commit_message>
FIX: Corrected the Reallocation Sheet
</commit_message>
<xml_diff>
--- a/test-data/SGA Budget Review Jan 25 2026.xlsx
+++ b/test-data/SGA Budget Review Jan 25 2026.xlsx
@@ -1,18 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A34424B-0705-8446-84FE-CFF94C84F4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="100" yWindow="680" windowWidth="30040" windowHeight="17680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="AFR Requests" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Reallocation Requests" state="visible" r:id="rId5"/>
+    <sheet name="AFR Requests" sheetId="1" r:id="rId1"/>
+    <sheet name="Reallocation Requests" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>Spring 2026</t>
   </si>
@@ -65,72 +82,81 @@
     <t>SGA 1</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Weekly Subtotal:</t>
+  </si>
+  <si>
+    <t>Remaining Budget:</t>
+  </si>
+  <si>
+    <t>Spring 2026 - Reallocations</t>
+  </si>
+  <si>
+    <t>Requested Amount</t>
+  </si>
+  <si>
+    <t>Approved Amount</t>
+  </si>
+  <si>
     <t>SGA 2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Weekly Subtotal:</t>
-  </si>
-  <si>
-    <t>Remaining Budget:</t>
-  </si>
-  <si>
-    <t>Spring 2026 - Reallocations</t>
-  </si>
-  <si>
-    <t>Requested Amount</t>
-  </si>
-  <si>
-    <t>Approved Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <color rgb="A32638"/>
       <sz val="20"/>
+      <color rgb="FFA32638"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <color rgb="1E1E1E"/>
       <sz val="16"/>
+      <color rgb="FF1E1E1E"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <color rgb="FFFFFF"/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <color rgb="A32638"/>
       <sz val="14"/>
+      <color rgb="FFA32638"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <color rgb="333333"/>
       <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -142,22 +168,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="A32638"/>
+        <fgColor rgb="FFA32638"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="F5F5F5"/>
+        <fgColor rgb="FFF5F5F5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="D9E2F3"/>
+        <fgColor rgb="FFD9E2F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2CC"/>
+        <fgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -170,54 +196,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="D0D0D0"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="D0D0D0"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="D0D0D0"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="D0D0D0"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="4472C4"/>
+        <color rgb="FFD0D0D0"/>
       </left>
       <right style="thin">
-        <color rgb="4472C4"/>
+        <color rgb="FFD0D0D0"/>
       </right>
-      <top style="medium">
-        <color rgb="4472C4"/>
+      <top style="thin">
+        <color rgb="FFD0D0D0"/>
       </top>
       <bottom style="thin">
-        <color rgb="4472C4"/>
+        <color rgb="FFD0D0D0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="DFA500"/>
+        <color rgb="FF4472C4"/>
       </left>
       <right style="thin">
-        <color rgb="DFA500"/>
+        <color rgb="FF4472C4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF4472C4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4472C4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDFA500"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDFA500"/>
       </right>
       <top style="thin">
-        <color rgb="DFA500"/>
+        <color rgb="FFDFA500"/>
       </top>
       <bottom style="medium">
-        <color rgb="DFA500"/>
+        <color rgb="FFDFA500"/>
       </bottom>
       <diagonal/>
     </border>
@@ -225,23 +259,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -260,6 +285,12 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,15 +630,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -623,216 +654,184 @@
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="2" ht="22" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="24" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
+        <v>551</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5-F5</f>
+        <v>551</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5">
+        <f>IF(G5="Approved",F5,0)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="8">
-        <f>D5-F5</f>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8">
-        <f>IF(G5="Approved",F5,0)</f>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>15</v>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8">
-        <v>551</v>
-      </c>
-      <c r="E6" s="8">
-        <f>D6-F6</f>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="8">
-        <f>IF(G6="Approved",F6,0)</f>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="7" t="s">
+    <row r="6" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="H6" s="7">
+        <f>SUM(H5:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" ht="22" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="9" t="s">
+    <row r="7" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="10">
-        <f>SUM(H5:H6)</f>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="26" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="12">
-        <f>I1-H7</f>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="H7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="9">
+        <f>I1-H6</f>
+        <v>100000</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -842,64 +841,78 @@
     <mergeCell ref="A4:L4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Status" error="Please select either Approved or Denied" sqref="G5:G6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Status" error="Please select either Approved or Denied" sqref="G5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Approved,Denied"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" ht="22" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
+      <c r="C3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -907,6 +920,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>